<commit_message>
26 sept 2019 intan accbid ubahprofil yg tak sempurna ini
</commit_message>
<xml_diff>
--- a/ubahprofil.xlsx
+++ b/ubahprofil.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intan\git\acctesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intan\git\ACCBid-Mobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
-  <si>
-    <t>nomorhandphone</t>
-  </si>
-  <si>
-    <t>tanggallahir</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>alamat</t>
   </si>
@@ -41,28 +35,46 @@
     <t>passed</t>
   </si>
   <si>
-    <t xml:space="preserve">jl kutai timur </t>
-  </si>
-  <si>
-    <t>expected</t>
-  </si>
-  <si>
-    <t>keterangan</t>
-  </si>
-  <si>
     <t>dokter</t>
   </si>
   <si>
     <t>failed</t>
   </si>
   <si>
-    <t>nomorterpakai</t>
-  </si>
-  <si>
-    <t>aaaaaaaaa</t>
-  </si>
-  <si>
-    <t>nomorharusnumerik</t>
+    <t>nomorhp</t>
+  </si>
+  <si>
+    <t>nomorhpexpected</t>
+  </si>
+  <si>
+    <t>varTahun</t>
+  </si>
+  <si>
+    <t>alamatexpected</t>
+  </si>
+  <si>
+    <t>pekerjaanexpected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected </t>
+  </si>
+  <si>
+    <t>jl nuri 30</t>
+  </si>
+  <si>
+    <t>mahasiswa</t>
+  </si>
+  <si>
+    <t>jl gagak 50</t>
+  </si>
+  <si>
+    <t>087830815asd</t>
+  </si>
+  <si>
+    <t>jl merpati 12</t>
+  </si>
+  <si>
+    <t>guru</t>
   </si>
 </sst>
 </file>
@@ -381,88 +393,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>87830815038</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="B2">
+        <v>87830815038</v>
+      </c>
+      <c r="C2">
+        <v>1997</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>81904067865</v>
+      </c>
+      <c r="B3">
+        <v>81904067865</v>
+      </c>
+      <c r="C3">
+        <v>1998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>87830815038</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>87830815</v>
+      </c>
+      <c r="C4">
+        <v>1998</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ubah profil 3 okt 2019
</commit_message>
<xml_diff>
--- a/ubahprofil.xlsx
+++ b/ubahprofil.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>alamat</t>
   </si>
@@ -59,22 +59,40 @@
     <t xml:space="preserve">expected </t>
   </si>
   <si>
-    <t>jl nuri 30</t>
-  </si>
-  <si>
     <t>mahasiswa</t>
   </si>
   <si>
     <t>jl gagak 50</t>
   </si>
   <si>
-    <t>087830815asd</t>
-  </si>
-  <si>
     <t>jl merpati 12</t>
   </si>
   <si>
     <t>guru</t>
+  </si>
+  <si>
+    <t>expected_nohp</t>
+  </si>
+  <si>
+    <t>jl kenangan 3</t>
+  </si>
+  <si>
+    <t>jl, neraka 7</t>
+  </si>
+  <si>
+    <t>pembantu</t>
+  </si>
+  <si>
+    <t>expected_alamat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected_pekerjaan </t>
+  </si>
+  <si>
+    <t>081asd</t>
+  </si>
+  <si>
+    <t>dokter?</t>
   </si>
 </sst>
 </file>
@@ -393,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,9 +427,12 @@
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -436,8 +457,17 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>87830815038</v>
       </c>
@@ -448,10 +478,10 @@
         <v>1997</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -462,56 +492,153 @@
       <c r="H2" t="s">
         <v>2</v>
       </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>81904067865</v>
+        <v>81225672116</v>
       </c>
       <c r="B3">
-        <v>81904067865</v>
+        <v>81225672116</v>
       </c>
       <c r="C3">
         <v>1998</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
       </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>87830815</v>
+        <v>81</v>
       </c>
       <c r="C4">
         <v>1998</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>87830815038</v>
+      </c>
+      <c r="B5">
+        <v>87830815038</v>
+      </c>
+      <c r="C5">
+        <v>1998</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>87830815038</v>
+      </c>
+      <c r="B6">
+        <v>87830815038</v>
+      </c>
+      <c r="C6">
+        <v>1998</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>